<commit_message>
Tiep tuc lam Data Cleaning
</commit_message>
<xml_diff>
--- a/dataset_giaxemaycu.xlsx
+++ b/dataset_giaxemaycu.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21522512_ms_uit_edu_vn/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_C1365E6BAA1B8F33E4D67E896E6F24CEFFED82A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2341B996-1440-418A-94B6-9D14433C2F06}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_giaxemaycu - dataset" sheetId="2" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'dataset_giaxemaycu - dataset'!$A$1:$Q$220</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,15 +33,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - dataset_giaxemaycu - dataset" description="Connection to the 'dataset_giaxemaycu - dataset' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Query - dataset_giaxemaycu - dataset" description="Connection to the 'dataset_giaxemaycu - dataset' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;dataset_giaxemaycu - dataset&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [dataset_giaxemaycu - dataset]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3074" uniqueCount="631">
   <si>
     <t>Hãng xe</t>
   </si>
@@ -1207,9 +1201,6 @@
     <t>Honda Super Cub C125</t>
   </si>
   <si>
-    <t>123,94</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -1273,9 +1264,6 @@
     <t>Honda SH 350i</t>
   </si>
   <si>
-    <t>329,6</t>
-  </si>
-  <si>
     <t>Honda Wave A 2022</t>
   </si>
   <si>
@@ -1402,9 +1390,6 @@
     <t>Honda sh 150i ABS 2021</t>
   </si>
   <si>
-    <t>156,9</t>
-  </si>
-  <si>
     <t>Honda Air Blade</t>
   </si>
   <si>
@@ -1516,9 +1501,6 @@
     <t xml:space="preserve">SH 300i </t>
   </si>
   <si>
-    <t>0,9</t>
-  </si>
-  <si>
     <t>4999</t>
   </si>
   <si>
@@ -1591,15 +1573,9 @@
     <t>Honda Wave Alpha 110cc</t>
   </si>
   <si>
-    <t>109,2</t>
-  </si>
-  <si>
     <t>Honda Vision 2016</t>
   </si>
   <si>
-    <t>11,3</t>
-  </si>
-  <si>
     <t>Honda VARIO 160</t>
   </si>
   <si>
@@ -1690,9 +1666,6 @@
     <t>Honda SH 125i</t>
   </si>
   <si>
-    <t>124,8</t>
-  </si>
-  <si>
     <t>Yamaha NVX 155</t>
   </si>
   <si>
@@ -1817,9 +1790,6 @@
   </si>
   <si>
     <t>3.6</t>
-  </si>
-  <si>
-    <t>49,95</t>
   </si>
   <si>
     <t>Honda Wave Alpha</t>
@@ -1969,7 +1939,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2070,7 +2040,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="18">
     <queryTableFields count="17">
       <queryTableField id="1" name="Hãng xe" tableColumnId="1"/>
@@ -2096,26 +2066,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="dataset_giaxemaycu___dataset" displayName="dataset_giaxemaycu___dataset" ref="A1:Q220" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Q220" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="dataset_giaxemaycu___dataset" displayName="dataset_giaxemaycu___dataset" ref="A1:Q220" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Q220"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Hãng xe" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Trọng lượng" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Mã lực" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Màu xe" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Năm sản xuất" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Dòng xe" queryTableFieldId="6" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Loại xe" queryTableFieldId="7" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="Tên xe" queryTableFieldId="8" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="Giá bán" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="Năm đăng ký" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" uniqueName="11" name="Tình trạng" queryTableFieldId="11" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="12" name="Dung Tích" queryTableFieldId="12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name="Xuất xứ" queryTableFieldId="13" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="14" name="Số km đã đi" queryTableFieldId="14" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="15" name="Chính sách bảo hành" queryTableFieldId="15" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" uniqueName="16" name="Giấy tờ" queryTableFieldId="16" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" uniqueName="17" name="Địa chỉ người bán" queryTableFieldId="17" dataDxfId="0"/>
+    <tableColumn id="1" uniqueName="1" name="Hãng xe" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" uniqueName="2" name="Trọng lượng" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" uniqueName="3" name="Mã lực" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" uniqueName="4" name="Màu xe" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" uniqueName="5" name="Năm sản xuất" queryTableFieldId="5"/>
+    <tableColumn id="6" uniqueName="6" name="Dòng xe" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="7" uniqueName="7" name="Loại xe" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="8" uniqueName="8" name="Tên xe" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="9" uniqueName="9" name="Giá bán" queryTableFieldId="9"/>
+    <tableColumn id="10" uniqueName="10" name="Năm đăng ký" queryTableFieldId="10"/>
+    <tableColumn id="11" uniqueName="11" name="Tình trạng" queryTableFieldId="11" dataDxfId="6"/>
+    <tableColumn id="12" uniqueName="12" name="Dung Tích" queryTableFieldId="12" dataDxfId="5"/>
+    <tableColumn id="13" uniqueName="13" name="Xuất xứ" queryTableFieldId="13" dataDxfId="4"/>
+    <tableColumn id="14" uniqueName="14" name="Số km đã đi" queryTableFieldId="14" dataDxfId="3"/>
+    <tableColumn id="15" uniqueName="15" name="Chính sách bảo hành" queryTableFieldId="15" dataDxfId="2"/>
+    <tableColumn id="16" uniqueName="16" name="Giấy tờ" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="17" uniqueName="17" name="Địa chỉ người bán" queryTableFieldId="17" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2410,17 +2380,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7141,14 +7113,14 @@
       <c r="K89" t="s">
         <v>73</v>
       </c>
-      <c r="L89" t="s">
-        <v>386</v>
+      <c r="L89">
+        <v>123.94</v>
       </c>
       <c r="M89" t="s">
         <v>123</v>
       </c>
       <c r="N89" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O89" t="s">
         <v>28</v>
@@ -7168,22 +7140,22 @@
         <v>221</v>
       </c>
       <c r="C90" t="s">
+        <v>387</v>
+      </c>
+      <c r="D90" t="s">
         <v>388</v>
-      </c>
-      <c r="D90" t="s">
-        <v>389</v>
       </c>
       <c r="E90">
         <v>2013</v>
       </c>
       <c r="F90" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G90" t="s">
         <v>36</v>
       </c>
       <c r="H90" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I90">
         <v>15000000</v>
@@ -7221,7 +7193,7 @@
         <v>63</v>
       </c>
       <c r="C91" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D91" t="s">
         <v>112</v>
@@ -7230,13 +7202,13 @@
         <v>2010</v>
       </c>
       <c r="F91" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G91" t="s">
         <v>36</v>
       </c>
       <c r="H91" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I91">
         <v>89000000</v>
@@ -7254,7 +7226,7 @@
         <v>26</v>
       </c>
       <c r="N91" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O91" t="s">
         <v>138</v>
@@ -7274,7 +7246,7 @@
         <v>163</v>
       </c>
       <c r="C92" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D92" t="s">
         <v>20</v>
@@ -7289,7 +7261,7 @@
         <v>247</v>
       </c>
       <c r="H92" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I92">
         <v>23500000</v>
@@ -7304,10 +7276,10 @@
         <v>163</v>
       </c>
       <c r="M92" t="s">
+        <v>397</v>
+      </c>
+      <c r="N92" t="s">
         <v>398</v>
-      </c>
-      <c r="N92" t="s">
-        <v>399</v>
       </c>
       <c r="O92" t="s">
         <v>99</v>
@@ -7324,10 +7296,10 @@
         <v>31</v>
       </c>
       <c r="B93" t="s">
+        <v>399</v>
+      </c>
+      <c r="C93" t="s">
         <v>400</v>
-      </c>
-      <c r="C93" t="s">
-        <v>401</v>
       </c>
       <c r="D93" t="s">
         <v>45</v>
@@ -7342,7 +7314,7 @@
         <v>36</v>
       </c>
       <c r="H93" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I93">
         <v>82000000</v>
@@ -7351,7 +7323,7 @@
         <v>2020</v>
       </c>
       <c r="K93" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L93" t="s">
         <v>105</v>
@@ -7377,10 +7349,10 @@
         <v>31</v>
       </c>
       <c r="B94" t="s">
+        <v>403</v>
+      </c>
+      <c r="C94" t="s">
         <v>404</v>
-      </c>
-      <c r="C94" t="s">
-        <v>405</v>
       </c>
       <c r="D94" t="s">
         <v>77</v>
@@ -7389,13 +7361,13 @@
         <v>2022</v>
       </c>
       <c r="F94" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G94" t="s">
         <v>36</v>
       </c>
       <c r="H94" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I94">
         <v>115000000</v>
@@ -7406,8 +7378,8 @@
       <c r="K94" t="s">
         <v>73</v>
       </c>
-      <c r="L94" t="s">
-        <v>408</v>
+      <c r="L94">
+        <v>329.6</v>
       </c>
       <c r="M94" t="s">
         <v>123</v>
@@ -7448,7 +7420,7 @@
         <v>47</v>
       </c>
       <c r="H95" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I95">
         <v>15500000</v>
@@ -7466,7 +7438,7 @@
         <v>40</v>
       </c>
       <c r="N95" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O95" t="s">
         <v>28</v>
@@ -7495,13 +7467,13 @@
         <v>2015</v>
       </c>
       <c r="F96" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G96" t="s">
         <v>36</v>
       </c>
       <c r="H96" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I96">
         <v>29800000</v>
@@ -7519,7 +7491,7 @@
         <v>26</v>
       </c>
       <c r="N96" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O96" t="s">
         <v>138</v>
@@ -7536,10 +7508,10 @@
         <v>284</v>
       </c>
       <c r="B97" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C97" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D97" t="s">
         <v>34</v>
@@ -7554,7 +7526,7 @@
         <v>36</v>
       </c>
       <c r="H97" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I97">
         <v>24500000</v>
@@ -7601,13 +7573,13 @@
         <v>2019</v>
       </c>
       <c r="F98" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G98" t="s">
         <v>22</v>
       </c>
       <c r="H98" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I98">
         <v>33500000</v>
@@ -7619,7 +7591,7 @@
         <v>24</v>
       </c>
       <c r="L98" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="M98" t="s">
         <v>106</v>
@@ -7660,7 +7632,7 @@
         <v>36</v>
       </c>
       <c r="H99" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I99">
         <v>39900000</v>
@@ -7713,7 +7685,7 @@
         <v>36</v>
       </c>
       <c r="H100" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I100">
         <v>29900000</v>
@@ -7760,13 +7732,13 @@
         <v>2019</v>
       </c>
       <c r="F101" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G101" t="s">
         <v>247</v>
       </c>
       <c r="H101" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I101">
         <v>14500000</v>
@@ -7784,7 +7756,7 @@
         <v>97</v>
       </c>
       <c r="N101" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="O101" t="s">
         <v>99</v>
@@ -7813,7 +7785,7 @@
         <v>2019</v>
       </c>
       <c r="F102" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G102" t="s">
         <v>94</v>
@@ -7837,7 +7809,7 @@
         <v>97</v>
       </c>
       <c r="N102" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="O102" t="s">
         <v>99</v>
@@ -7857,7 +7829,7 @@
         <v>184</v>
       </c>
       <c r="C103" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D103" t="s">
         <v>20</v>
@@ -7872,7 +7844,7 @@
         <v>47</v>
       </c>
       <c r="H103" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I103">
         <v>13500000</v>
@@ -7910,7 +7882,7 @@
         <v>150</v>
       </c>
       <c r="C104" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D104" t="s">
         <v>45</v>
@@ -7925,7 +7897,7 @@
         <v>22</v>
       </c>
       <c r="H104" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I104">
         <v>23500000</v>
@@ -7943,7 +7915,7 @@
         <v>40</v>
       </c>
       <c r="N104" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="O104" t="s">
         <v>28</v>
@@ -7960,7 +7932,7 @@
         <v>31</v>
       </c>
       <c r="B105" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C105" t="s">
         <v>300</v>
@@ -7978,7 +7950,7 @@
         <v>47</v>
       </c>
       <c r="H105" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I105">
         <v>31000000</v>
@@ -7996,7 +7968,7 @@
         <v>40</v>
       </c>
       <c r="N105" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="O105" t="s">
         <v>28</v>
@@ -8016,7 +7988,7 @@
         <v>158</v>
       </c>
       <c r="C106" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D106" t="s">
         <v>180</v>
@@ -8031,7 +8003,7 @@
         <v>380</v>
       </c>
       <c r="H106" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I106">
         <v>23500000</v>
@@ -8049,7 +8021,7 @@
         <v>40</v>
       </c>
       <c r="N106" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O106" t="s">
         <v>28</v>
@@ -8078,13 +8050,13 @@
         <v>2018</v>
       </c>
       <c r="F107" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G107" t="s">
         <v>36</v>
       </c>
       <c r="H107" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I107">
         <v>36800000</v>
@@ -8137,7 +8109,7 @@
         <v>36</v>
       </c>
       <c r="H108" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I108">
         <v>20000000</v>
@@ -8155,7 +8127,7 @@
         <v>26</v>
       </c>
       <c r="N108" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="O108" t="s">
         <v>28</v>
@@ -8175,7 +8147,7 @@
         <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D109" t="s">
         <v>45</v>
@@ -8190,7 +8162,7 @@
         <v>380</v>
       </c>
       <c r="H109" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I109">
         <v>22500000</v>
@@ -8270,7 +8242,7 @@
         <v>108</v>
       </c>
       <c r="Q110" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.35">
@@ -8349,7 +8321,7 @@
         <v>22</v>
       </c>
       <c r="H112" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I112">
         <v>24800000</v>
@@ -8367,7 +8339,7 @@
         <v>97</v>
       </c>
       <c r="N112" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O112" t="s">
         <v>250</v>
@@ -8402,7 +8374,7 @@
         <v>36</v>
       </c>
       <c r="H113" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I113">
         <v>11500000</v>
@@ -8420,7 +8392,7 @@
         <v>84</v>
       </c>
       <c r="N113" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O113" t="s">
         <v>28</v>
@@ -8429,7 +8401,7 @@
         <v>108</v>
       </c>
       <c r="Q113" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.35">
@@ -8455,7 +8427,7 @@
         <v>36</v>
       </c>
       <c r="H114" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I114">
         <v>34000000</v>
@@ -8473,7 +8445,7 @@
         <v>26</v>
       </c>
       <c r="N114" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O114" t="s">
         <v>28</v>
@@ -8490,10 +8462,10 @@
         <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C115" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D115" t="s">
         <v>112</v>
@@ -8502,13 +8474,13 @@
         <v>2023</v>
       </c>
       <c r="F115" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G115" t="s">
         <v>36</v>
       </c>
       <c r="H115" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I115">
         <v>84000000</v>
@@ -8526,7 +8498,7 @@
         <v>26</v>
       </c>
       <c r="N115" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="O115" t="s">
         <v>28</v>
@@ -8561,7 +8533,7 @@
         <v>47</v>
       </c>
       <c r="H116" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I116">
         <v>5300000</v>
@@ -8632,7 +8604,7 @@
         <v>40</v>
       </c>
       <c r="N117" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O117" t="s">
         <v>28</v>
@@ -8714,13 +8686,13 @@
         <v>2021</v>
       </c>
       <c r="F119" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G119" t="s">
         <v>36</v>
       </c>
       <c r="H119" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I119">
         <v>82000000</v>
@@ -8731,8 +8703,8 @@
       <c r="K119" t="s">
         <v>60</v>
       </c>
-      <c r="L119" t="s">
-        <v>451</v>
+      <c r="L119">
+        <v>156.9</v>
       </c>
       <c r="M119" t="s">
         <v>40</v>
@@ -8758,7 +8730,7 @@
         <v>32</v>
       </c>
       <c r="C120" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D120" t="s">
         <v>77</v>
@@ -8773,7 +8745,7 @@
         <v>36</v>
       </c>
       <c r="H120" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I120">
         <v>38500000</v>
@@ -8791,7 +8763,7 @@
         <v>26</v>
       </c>
       <c r="N120" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="O120" t="s">
         <v>28</v>
@@ -8808,10 +8780,10 @@
         <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C121" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D121" t="s">
         <v>77</v>
@@ -8826,7 +8798,7 @@
         <v>22</v>
       </c>
       <c r="H121" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I121">
         <v>120000000</v>
@@ -8835,16 +8807,16 @@
         <v>2017</v>
       </c>
       <c r="K121" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="L121" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="M121" t="s">
         <v>40</v>
       </c>
       <c r="N121" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="O121" t="s">
         <v>138</v>
@@ -8861,13 +8833,13 @@
         <v>31</v>
       </c>
       <c r="B122" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C122" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D122" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E122">
         <v>2010</v>
@@ -8879,7 +8851,7 @@
         <v>36</v>
       </c>
       <c r="H122" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="I122">
         <v>8500000</v>
@@ -8917,7 +8889,7 @@
         <v>244</v>
       </c>
       <c r="C123" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D123" t="s">
         <v>112</v>
@@ -8932,7 +8904,7 @@
         <v>47</v>
       </c>
       <c r="H123" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I123">
         <v>11500000</v>
@@ -8950,7 +8922,7 @@
         <v>84</v>
       </c>
       <c r="N123" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="O123" t="s">
         <v>28</v>
@@ -8970,7 +8942,7 @@
         <v>63</v>
       </c>
       <c r="C124" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D124" t="s">
         <v>77</v>
@@ -8985,7 +8957,7 @@
         <v>22</v>
       </c>
       <c r="H124" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I124">
         <v>34800000</v>
@@ -9003,7 +8975,7 @@
         <v>40</v>
       </c>
       <c r="N124" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="O124" t="s">
         <v>28</v>
@@ -9091,7 +9063,7 @@
         <v>36</v>
       </c>
       <c r="H126" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I126">
         <v>40500000</v>
@@ -9126,7 +9098,7 @@
         <v>284</v>
       </c>
       <c r="B127" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C127" t="s">
         <v>33</v>
@@ -9144,7 +9116,7 @@
         <v>36</v>
       </c>
       <c r="H127" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I127">
         <v>8500000</v>
@@ -9159,10 +9131,10 @@
         <v>39</v>
       </c>
       <c r="M127" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="N127" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="O127" t="s">
         <v>28</v>
@@ -9185,7 +9157,7 @@
         <v>170</v>
       </c>
       <c r="D128" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E128">
         <v>2016</v>
@@ -9197,7 +9169,7 @@
         <v>247</v>
       </c>
       <c r="H128" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I128">
         <v>14800000</v>
@@ -9235,7 +9207,7 @@
         <v>43</v>
       </c>
       <c r="C129" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D129" t="s">
         <v>112</v>
@@ -9250,7 +9222,7 @@
         <v>47</v>
       </c>
       <c r="H129" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I129">
         <v>1700000</v>
@@ -9259,7 +9231,7 @@
         <v>2022</v>
       </c>
       <c r="K129" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="L129" t="s">
         <v>32</v>
@@ -9303,7 +9275,7 @@
         <v>22</v>
       </c>
       <c r="H130" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I130">
         <v>24000000</v>
@@ -9356,7 +9328,7 @@
         <v>36</v>
       </c>
       <c r="H131" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I131">
         <v>36800000</v>
@@ -9447,7 +9419,7 @@
         <v>184</v>
       </c>
       <c r="C133" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D133" t="s">
         <v>20</v>
@@ -9462,7 +9434,7 @@
         <v>47</v>
       </c>
       <c r="H133" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I133">
         <v>14500000</v>
@@ -9480,7 +9452,7 @@
         <v>26</v>
       </c>
       <c r="N133" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="O133" t="s">
         <v>138</v>
@@ -9500,7 +9472,7 @@
         <v>128</v>
       </c>
       <c r="C134" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D134" t="s">
         <v>112</v>
@@ -9509,13 +9481,13 @@
         <v>2009</v>
       </c>
       <c r="F134" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G134" t="s">
         <v>36</v>
       </c>
       <c r="H134" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I134">
         <v>3500000</v>
@@ -9527,7 +9499,7 @@
         <v>297</v>
       </c>
       <c r="L134" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="M134" t="s">
         <v>287</v>
@@ -9568,7 +9540,7 @@
         <v>47</v>
       </c>
       <c r="H135" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I135">
         <v>24000000</v>
@@ -9621,7 +9593,7 @@
         <v>22</v>
       </c>
       <c r="H136" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I136">
         <v>23500000</v>
@@ -9630,7 +9602,7 @@
         <v>2017</v>
       </c>
       <c r="K136" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="L136" t="s">
         <v>182</v>
@@ -9639,7 +9611,7 @@
         <v>26</v>
       </c>
       <c r="N136" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O136" t="s">
         <v>138</v>
@@ -9674,7 +9646,7 @@
         <v>36</v>
       </c>
       <c r="H137" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I137">
         <v>40000000</v>
@@ -9701,7 +9673,7 @@
         <v>29</v>
       </c>
       <c r="Q137" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.35">
@@ -9727,7 +9699,7 @@
         <v>254</v>
       </c>
       <c r="H138" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I138">
         <v>128000000</v>
@@ -9735,20 +9707,20 @@
       <c r="J138">
         <v>2022</v>
       </c>
-      <c r="K138" t="s">
-        <v>489</v>
+      <c r="K138">
+        <v>0.9</v>
       </c>
       <c r="L138" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="M138" t="s">
         <v>123</v>
       </c>
       <c r="N138" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="O138" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="P138" t="s">
         <v>108</v>
@@ -9780,7 +9752,7 @@
         <v>36</v>
       </c>
       <c r="H139" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I139">
         <v>45000000</v>
@@ -9871,7 +9843,7 @@
         <v>43</v>
       </c>
       <c r="C141" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D141" t="s">
         <v>112</v>
@@ -9886,7 +9858,7 @@
         <v>47</v>
       </c>
       <c r="H141" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I141">
         <v>6500000</v>
@@ -9904,7 +9876,7 @@
         <v>40</v>
       </c>
       <c r="N141" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="O141" t="s">
         <v>138</v>
@@ -9921,10 +9893,10 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C142" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D142" t="s">
         <v>45</v>
@@ -9933,13 +9905,13 @@
         <v>2022</v>
       </c>
       <c r="F142" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G142" t="s">
         <v>22</v>
       </c>
       <c r="H142" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I142">
         <v>70000000</v>
@@ -9951,7 +9923,7 @@
         <v>104</v>
       </c>
       <c r="L142" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="M142" t="s">
         <v>40</v>
@@ -9977,7 +9949,7 @@
         <v>110</v>
       </c>
       <c r="C143" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D143" t="s">
         <v>112</v>
@@ -9992,7 +9964,7 @@
         <v>36</v>
       </c>
       <c r="H143" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="I143">
         <v>75000000</v>
@@ -10030,7 +10002,7 @@
         <v>43</v>
       </c>
       <c r="C144" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D144" t="s">
         <v>77</v>
@@ -10045,7 +10017,7 @@
         <v>47</v>
       </c>
       <c r="H144" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="I144">
         <v>9000000</v>
@@ -10057,13 +10029,13 @@
         <v>175</v>
       </c>
       <c r="L144" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="M144" t="s">
         <v>26</v>
       </c>
       <c r="N144" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="O144" t="s">
         <v>138</v>
@@ -10083,7 +10055,7 @@
         <v>32</v>
       </c>
       <c r="C145" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D145" t="s">
         <v>77</v>
@@ -10098,7 +10070,7 @@
         <v>36</v>
       </c>
       <c r="H145" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I145">
         <v>22500000</v>
@@ -10116,7 +10088,7 @@
         <v>26</v>
       </c>
       <c r="N145" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="O145" t="s">
         <v>28</v>
@@ -10136,7 +10108,7 @@
         <v>43</v>
       </c>
       <c r="C146" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D146" t="s">
         <v>77</v>
@@ -10151,7 +10123,7 @@
         <v>47</v>
       </c>
       <c r="H146" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I146">
         <v>12200000</v>
@@ -10178,7 +10150,7 @@
         <v>29</v>
       </c>
       <c r="Q146" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.35">
@@ -10204,7 +10176,7 @@
         <v>36</v>
       </c>
       <c r="H147" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I147">
         <v>39000000</v>
@@ -10222,7 +10194,7 @@
         <v>26</v>
       </c>
       <c r="N147" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="O147" t="s">
         <v>28</v>
@@ -10257,7 +10229,7 @@
         <v>47</v>
       </c>
       <c r="H148" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I148">
         <v>14900000</v>
@@ -10275,7 +10247,7 @@
         <v>40</v>
       </c>
       <c r="N148" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="O148" t="s">
         <v>28</v>
@@ -10310,7 +10282,7 @@
         <v>47</v>
       </c>
       <c r="H149" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="I149">
         <v>9800000</v>
@@ -10321,8 +10293,8 @@
       <c r="K149" t="s">
         <v>24</v>
       </c>
-      <c r="L149" t="s">
-        <v>514</v>
+      <c r="L149">
+        <v>109.2</v>
       </c>
       <c r="M149" t="s">
         <v>40</v>
@@ -10363,7 +10335,7 @@
         <v>36</v>
       </c>
       <c r="H150" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I150">
         <v>22500000</v>
@@ -10400,8 +10372,8 @@
       <c r="B151" t="s">
         <v>18</v>
       </c>
-      <c r="C151" t="s">
-        <v>516</v>
+      <c r="C151">
+        <v>11.3</v>
       </c>
       <c r="D151" t="s">
         <v>34</v>
@@ -10416,7 +10388,7 @@
         <v>22</v>
       </c>
       <c r="H151" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="I151">
         <v>44500000</v>
@@ -10427,14 +10399,14 @@
       <c r="K151" t="s">
         <v>73</v>
       </c>
-      <c r="L151" t="s">
-        <v>451</v>
+      <c r="L151">
+        <v>156.9</v>
       </c>
       <c r="M151" t="s">
         <v>40</v>
       </c>
       <c r="N151" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O151" t="s">
         <v>28</v>
@@ -10487,7 +10459,7 @@
         <v>26</v>
       </c>
       <c r="N152" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O152" t="s">
         <v>28</v>
@@ -10496,7 +10468,7 @@
         <v>29</v>
       </c>
       <c r="Q152" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.35">
@@ -10522,7 +10494,7 @@
         <v>47</v>
       </c>
       <c r="H153" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="I153">
         <v>9700000</v>
@@ -10534,13 +10506,13 @@
         <v>175</v>
       </c>
       <c r="L153" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="M153" t="s">
         <v>84</v>
       </c>
       <c r="N153" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="O153" t="s">
         <v>138</v>
@@ -10569,13 +10541,13 @@
         <v>2022</v>
       </c>
       <c r="F154" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="G154" t="s">
         <v>94</v>
       </c>
       <c r="H154" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="I154">
         <v>32800000</v>
@@ -10628,7 +10600,7 @@
         <v>36</v>
       </c>
       <c r="H155" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="I155">
         <v>21500000</v>
@@ -10681,7 +10653,7 @@
         <v>47</v>
       </c>
       <c r="H156" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="I156">
         <v>12000000</v>
@@ -10734,7 +10706,7 @@
         <v>47</v>
       </c>
       <c r="H157" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="I157">
         <v>12500000</v>
@@ -10772,7 +10744,7 @@
         <v>228</v>
       </c>
       <c r="C158" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D158" t="s">
         <v>65</v>
@@ -10781,13 +10753,13 @@
         <v>2022</v>
       </c>
       <c r="F158" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="G158" t="s">
         <v>22</v>
       </c>
       <c r="H158" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="I158">
         <v>23800000</v>
@@ -10805,7 +10777,7 @@
         <v>106</v>
       </c>
       <c r="N158" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="O158" t="s">
         <v>28</v>
@@ -10840,7 +10812,7 @@
         <v>22</v>
       </c>
       <c r="H159" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="I159">
         <v>23500000</v>
@@ -10855,10 +10827,10 @@
         <v>105</v>
       </c>
       <c r="M159" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="N159" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="O159" t="s">
         <v>28</v>
@@ -10875,7 +10847,7 @@
         <v>31</v>
       </c>
       <c r="B160" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C160" t="s">
         <v>328</v>
@@ -10893,7 +10865,7 @@
         <v>47</v>
       </c>
       <c r="H160" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="I160">
         <v>21000000</v>
@@ -10946,7 +10918,7 @@
         <v>47</v>
       </c>
       <c r="H161" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="I161">
         <v>20500000</v>
@@ -10984,7 +10956,7 @@
         <v>128</v>
       </c>
       <c r="C162" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D162" t="s">
         <v>45</v>
@@ -10999,7 +10971,7 @@
         <v>36</v>
       </c>
       <c r="H162" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="I162">
         <v>24500000</v>
@@ -11052,7 +11024,7 @@
         <v>36</v>
       </c>
       <c r="H163" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="I163">
         <v>28000000</v>
@@ -11070,7 +11042,7 @@
         <v>40</v>
       </c>
       <c r="N163" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="O163" t="s">
         <v>28</v>
@@ -11079,7 +11051,7 @@
         <v>29</v>
       </c>
       <c r="Q163" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.35">
@@ -11090,7 +11062,7 @@
         <v>172</v>
       </c>
       <c r="C164" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D164" t="s">
         <v>77</v>
@@ -11099,7 +11071,7 @@
         <v>2021</v>
       </c>
       <c r="F164" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G164" t="s">
         <v>36</v>
@@ -11152,13 +11124,13 @@
         <v>2008</v>
       </c>
       <c r="F165" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="G165" t="s">
         <v>36</v>
       </c>
       <c r="H165" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="I165">
         <v>12000000</v>
@@ -11185,7 +11157,7 @@
         <v>108</v>
       </c>
       <c r="Q165" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.35">
@@ -11211,7 +11183,7 @@
         <v>36</v>
       </c>
       <c r="H166" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="I166">
         <v>31500000</v>
@@ -11264,7 +11236,7 @@
         <v>36</v>
       </c>
       <c r="H167" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="I167">
         <v>43500000</v>
@@ -11273,7 +11245,7 @@
         <v>2023</v>
       </c>
       <c r="K167" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L167" t="s">
         <v>39</v>
@@ -11291,7 +11263,7 @@
         <v>29</v>
       </c>
       <c r="Q167" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.35">
@@ -11302,7 +11274,7 @@
         <v>110</v>
       </c>
       <c r="C168" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D168" t="s">
         <v>112</v>
@@ -11311,13 +11283,13 @@
         <v>2023</v>
       </c>
       <c r="F168" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G168" t="s">
         <v>36</v>
       </c>
       <c r="H168" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="I168">
         <v>62800000</v>
@@ -11328,8 +11300,8 @@
       <c r="K168" t="s">
         <v>73</v>
       </c>
-      <c r="L168" t="s">
-        <v>547</v>
+      <c r="L168">
+        <v>124.8</v>
       </c>
       <c r="M168" t="s">
         <v>40</v>
@@ -11370,7 +11342,7 @@
         <v>36</v>
       </c>
       <c r="H169" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="I169">
         <v>22500000</v>
@@ -11388,7 +11360,7 @@
         <v>40</v>
       </c>
       <c r="N169" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="O169" t="s">
         <v>28</v>
@@ -11423,7 +11395,7 @@
         <v>36</v>
       </c>
       <c r="H170" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="I170">
         <v>58000000</v>
@@ -11441,7 +11413,7 @@
         <v>97</v>
       </c>
       <c r="N170" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="O170" t="s">
         <v>99</v>
@@ -11529,7 +11501,7 @@
         <v>22</v>
       </c>
       <c r="H172" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I172">
         <v>12500000</v>
@@ -11541,7 +11513,7 @@
         <v>175</v>
       </c>
       <c r="L172" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="M172" t="s">
         <v>26</v>
@@ -11561,10 +11533,10 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="B173" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="C173" t="s">
         <v>84</v>
@@ -11582,7 +11554,7 @@
         <v>47</v>
       </c>
       <c r="H173" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="I173">
         <v>13000000</v>
@@ -11591,7 +11563,7 @@
         <v>1987</v>
       </c>
       <c r="K173" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="L173" t="s">
         <v>87</v>
@@ -11600,7 +11572,7 @@
         <v>40</v>
       </c>
       <c r="N173" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="O173" t="s">
         <v>138</v>
@@ -11623,7 +11595,7 @@
         <v>84</v>
       </c>
       <c r="D174" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="E174">
         <v>2011</v>
@@ -11635,7 +11607,7 @@
         <v>36</v>
       </c>
       <c r="H174" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="I174">
         <v>42500000</v>
@@ -11653,7 +11625,7 @@
         <v>123</v>
       </c>
       <c r="N174" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O174" t="s">
         <v>138</v>
@@ -11673,7 +11645,7 @@
         <v>43</v>
       </c>
       <c r="C175" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="D175" t="s">
         <v>77</v>
@@ -11688,7 +11660,7 @@
         <v>47</v>
       </c>
       <c r="H175" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="I175">
         <v>9000000</v>
@@ -11741,7 +11713,7 @@
         <v>36</v>
       </c>
       <c r="H176" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I176">
         <v>34500000</v>
@@ -11794,7 +11766,7 @@
         <v>247</v>
       </c>
       <c r="H177" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="I177">
         <v>6300000</v>
@@ -11865,7 +11837,7 @@
         <v>40</v>
       </c>
       <c r="N178" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="O178" t="s">
         <v>28</v>
@@ -11900,7 +11872,7 @@
         <v>36</v>
       </c>
       <c r="H179" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="I179">
         <v>39000000</v>
@@ -11938,7 +11910,7 @@
         <v>70</v>
       </c>
       <c r="C180" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D180" t="s">
         <v>20</v>
@@ -11953,7 +11925,7 @@
         <v>94</v>
       </c>
       <c r="H180" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="I180">
         <v>10500000</v>
@@ -11971,7 +11943,7 @@
         <v>276</v>
       </c>
       <c r="N180" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="O180" t="s">
         <v>99</v>
@@ -12006,7 +11978,7 @@
         <v>94</v>
       </c>
       <c r="H181" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="I181">
         <v>72900000</v>
@@ -12024,7 +11996,7 @@
         <v>97</v>
       </c>
       <c r="N181" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="O181" t="s">
         <v>250</v>
@@ -12044,7 +12016,7 @@
         <v>258</v>
       </c>
       <c r="C182" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="D182" t="s">
         <v>34</v>
@@ -12059,7 +12031,7 @@
         <v>22</v>
       </c>
       <c r="H182" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="I182">
         <v>29800000</v>
@@ -12074,13 +12046,13 @@
         <v>105</v>
       </c>
       <c r="M182" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="N182" t="s">
         <v>131</v>
       </c>
       <c r="O182" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="P182" t="s">
         <v>108</v>
@@ -12112,7 +12084,7 @@
         <v>36</v>
       </c>
       <c r="H183" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I183">
         <v>36000000</v>
@@ -12130,7 +12102,7 @@
         <v>84</v>
       </c>
       <c r="N183" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="O183" t="s">
         <v>28</v>
@@ -12165,7 +12137,7 @@
         <v>22</v>
       </c>
       <c r="H184" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I184">
         <v>20500000</v>
@@ -12183,7 +12155,7 @@
         <v>84</v>
       </c>
       <c r="N184" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="O184" t="s">
         <v>28</v>
@@ -12265,13 +12237,13 @@
         <v>2013</v>
       </c>
       <c r="F186" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G186" t="s">
         <v>36</v>
       </c>
       <c r="H186" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I186">
         <v>11300000</v>
@@ -12362,7 +12334,7 @@
         <v>172</v>
       </c>
       <c r="C188" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D188" t="s">
         <v>134</v>
@@ -12377,7 +12349,7 @@
         <v>47</v>
       </c>
       <c r="H188" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="I188">
         <v>11500000</v>
@@ -12415,10 +12387,10 @@
         <v>43</v>
       </c>
       <c r="C189" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D189" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="E189">
         <v>2018</v>
@@ -12430,7 +12402,7 @@
         <v>47</v>
       </c>
       <c r="H189" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="I189">
         <v>8800000</v>
@@ -12448,7 +12420,7 @@
         <v>84</v>
       </c>
       <c r="N189" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O189" t="s">
         <v>28</v>
@@ -12483,7 +12455,7 @@
         <v>94</v>
       </c>
       <c r="H190" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="I190">
         <v>18500000</v>
@@ -12501,7 +12473,7 @@
         <v>97</v>
       </c>
       <c r="N190" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="O190" t="s">
         <v>99</v>
@@ -12510,7 +12482,7 @@
         <v>100</v>
       </c>
       <c r="Q190" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.35">
@@ -12554,7 +12526,7 @@
         <v>40</v>
       </c>
       <c r="N191" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O191" t="s">
         <v>28</v>
@@ -12574,7 +12546,7 @@
         <v>178</v>
       </c>
       <c r="C192" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="D192" t="s">
         <v>20</v>
@@ -12586,10 +12558,10 @@
         <v>260</v>
       </c>
       <c r="G192" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="H192" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="I192">
         <v>18800000</v>
@@ -12695,7 +12667,7 @@
         <v>247</v>
       </c>
       <c r="H194" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="I194">
         <v>88000000</v>
@@ -12707,13 +12679,13 @@
         <v>315</v>
       </c>
       <c r="L194" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="M194" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N194" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="O194" t="s">
         <v>250</v>
@@ -12730,10 +12702,10 @@
         <v>17</v>
       </c>
       <c r="B195" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="C195" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="D195" t="s">
         <v>92</v>
@@ -12759,14 +12731,14 @@
       <c r="K195" t="s">
         <v>60</v>
       </c>
-      <c r="L195" t="s">
-        <v>590</v>
+      <c r="L195">
+        <v>49.95</v>
       </c>
       <c r="M195" t="s">
         <v>26</v>
       </c>
       <c r="N195" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O195" t="s">
         <v>28</v>
@@ -12801,7 +12773,7 @@
         <v>47</v>
       </c>
       <c r="H196" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="I196">
         <v>9700000</v>
@@ -12819,7 +12791,7 @@
         <v>84</v>
       </c>
       <c r="N196" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="O196" t="s">
         <v>138</v>
@@ -12854,7 +12826,7 @@
         <v>36</v>
       </c>
       <c r="H197" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="I197">
         <v>28800000</v>
@@ -12872,7 +12844,7 @@
         <v>40</v>
       </c>
       <c r="N197" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="O197" t="s">
         <v>28</v>
@@ -12901,13 +12873,13 @@
         <v>2020</v>
       </c>
       <c r="F198" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="G198" t="s">
         <v>94</v>
       </c>
       <c r="H198" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="I198">
         <v>58000000</v>
@@ -12925,7 +12897,7 @@
         <v>97</v>
       </c>
       <c r="N198" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O198" t="s">
         <v>250</v>
@@ -12945,7 +12917,7 @@
         <v>221</v>
       </c>
       <c r="C199" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="D199" t="s">
         <v>34</v>
@@ -12954,13 +12926,13 @@
         <v>2013</v>
       </c>
       <c r="F199" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G199" t="s">
         <v>36</v>
       </c>
       <c r="H199" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="I199">
         <v>8800000</v>
@@ -12978,7 +12950,7 @@
         <v>106</v>
       </c>
       <c r="N199" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O199" t="s">
         <v>28</v>
@@ -12998,7 +12970,7 @@
         <v>252</v>
       </c>
       <c r="C200" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="D200" t="s">
         <v>134</v>
@@ -13013,7 +12985,7 @@
         <v>36</v>
       </c>
       <c r="H200" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="I200">
         <v>39000000</v>
@@ -13051,7 +13023,7 @@
         <v>163</v>
       </c>
       <c r="C201" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D201" t="s">
         <v>20</v>
@@ -13066,7 +13038,7 @@
         <v>247</v>
       </c>
       <c r="H201" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="I201">
         <v>11500000</v>
@@ -13084,7 +13056,7 @@
         <v>97</v>
       </c>
       <c r="N201" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O201" t="s">
         <v>99</v>
@@ -13113,13 +13085,13 @@
         <v>2017</v>
       </c>
       <c r="F202" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="G202" t="s">
         <v>94</v>
       </c>
       <c r="H202" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="I202">
         <v>55000000</v>
@@ -13154,10 +13126,10 @@
         <v>83</v>
       </c>
       <c r="B203" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="C203" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="D203" t="s">
         <v>45</v>
@@ -13172,7 +13144,7 @@
         <v>47</v>
       </c>
       <c r="H203" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="I203">
         <v>13500000</v>
@@ -13190,7 +13162,7 @@
         <v>287</v>
       </c>
       <c r="N203" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="O203" t="s">
         <v>28</v>
@@ -13207,7 +13179,7 @@
         <v>31</v>
       </c>
       <c r="B204" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C204" t="s">
         <v>300</v>
@@ -13225,7 +13197,7 @@
         <v>47</v>
       </c>
       <c r="H204" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I204">
         <v>28500000</v>
@@ -13243,7 +13215,7 @@
         <v>40</v>
       </c>
       <c r="N204" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O204" t="s">
         <v>28</v>
@@ -13319,7 +13291,7 @@
         <v>199</v>
       </c>
       <c r="D206" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="E206">
         <v>2017</v>
@@ -13331,7 +13303,7 @@
         <v>36</v>
       </c>
       <c r="H206" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="I206">
         <v>55000000</v>
@@ -13349,7 +13321,7 @@
         <v>84</v>
       </c>
       <c r="N206" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O206" t="s">
         <v>28</v>
@@ -13422,7 +13394,7 @@
         <v>56</v>
       </c>
       <c r="C208" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D208" t="s">
         <v>112</v>
@@ -13437,7 +13409,7 @@
         <v>36</v>
       </c>
       <c r="H208" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="I208">
         <v>9600000</v>
@@ -13455,7 +13427,7 @@
         <v>84</v>
       </c>
       <c r="N208" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="O208" t="s">
         <v>28</v>
@@ -13464,7 +13436,7 @@
         <v>108</v>
       </c>
       <c r="Q208" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.35">
@@ -13484,13 +13456,13 @@
         <v>2017</v>
       </c>
       <c r="F209" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="G209" t="s">
         <v>22</v>
       </c>
       <c r="H209" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="I209">
         <v>14300000</v>
@@ -13502,7 +13474,7 @@
         <v>24</v>
       </c>
       <c r="L209" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="M209" t="s">
         <v>276</v>
@@ -13528,7 +13500,7 @@
         <v>184</v>
       </c>
       <c r="C210" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D210" t="s">
         <v>112</v>
@@ -13543,7 +13515,7 @@
         <v>47</v>
       </c>
       <c r="H210" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="I210">
         <v>8500000</v>
@@ -13561,7 +13533,7 @@
         <v>40</v>
       </c>
       <c r="N210" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="O210" t="s">
         <v>138</v>
@@ -13570,7 +13542,7 @@
         <v>81</v>
       </c>
       <c r="Q210" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.35">
@@ -13596,7 +13568,7 @@
         <v>36</v>
       </c>
       <c r="H211" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="I211">
         <v>16000000</v>
@@ -13614,7 +13586,7 @@
         <v>106</v>
       </c>
       <c r="N211" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="O211" t="s">
         <v>28</v>
@@ -13623,7 +13595,7 @@
         <v>108</v>
       </c>
       <c r="Q211" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.35">
@@ -13631,10 +13603,10 @@
         <v>83</v>
       </c>
       <c r="B212" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C212" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="D212" t="s">
         <v>20</v>
@@ -13643,13 +13615,13 @@
         <v>2019</v>
       </c>
       <c r="F212" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="G212" t="s">
         <v>47</v>
       </c>
       <c r="H212" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="I212">
         <v>10300000</v>
@@ -13673,7 +13645,7 @@
         <v>28</v>
       </c>
       <c r="P212" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="Q212" t="s">
         <v>69</v>
@@ -13702,7 +13674,7 @@
         <v>22</v>
       </c>
       <c r="H213" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="I213">
         <v>22500000</v>
@@ -13755,7 +13727,7 @@
         <v>36</v>
       </c>
       <c r="H214" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="I214">
         <v>20500000</v>
@@ -13773,7 +13745,7 @@
         <v>40</v>
       </c>
       <c r="N214" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O214" t="s">
         <v>28</v>
@@ -13793,7 +13765,7 @@
         <v>63</v>
       </c>
       <c r="C215" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="D215" t="s">
         <v>77</v>
@@ -13808,7 +13780,7 @@
         <v>254</v>
       </c>
       <c r="H215" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="I215">
         <v>299000000</v>
@@ -13820,13 +13792,13 @@
         <v>24</v>
       </c>
       <c r="L215" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="M215" t="s">
         <v>269</v>
       </c>
       <c r="N215" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="O215" t="s">
         <v>28</v>
@@ -13843,10 +13815,10 @@
         <v>31</v>
       </c>
       <c r="B216" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="C216" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="D216" t="s">
         <v>373</v>
@@ -13861,7 +13833,7 @@
         <v>36</v>
       </c>
       <c r="H216" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="I216">
         <v>23800000</v>
@@ -13914,7 +13886,7 @@
         <v>36</v>
       </c>
       <c r="H217" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="I217">
         <v>38800000</v>
@@ -13932,7 +13904,7 @@
         <v>40</v>
       </c>
       <c r="N217" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="O217" t="s">
         <v>28</v>
@@ -13949,10 +13921,10 @@
         <v>31</v>
       </c>
       <c r="B218" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C218" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="D218" t="s">
         <v>379</v>
@@ -13961,13 +13933,13 @@
         <v>2015</v>
       </c>
       <c r="F218" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="G218" t="s">
         <v>94</v>
       </c>
       <c r="H218" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="I218">
         <v>21500000</v>
@@ -13979,13 +13951,13 @@
         <v>38</v>
       </c>
       <c r="L218" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="M218" t="s">
         <v>97</v>
       </c>
       <c r="N218" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="O218" t="s">
         <v>99</v>
@@ -13994,7 +13966,7 @@
         <v>240</v>
       </c>
       <c r="Q218" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.35">
@@ -14020,7 +13992,7 @@
         <v>36</v>
       </c>
       <c r="H219" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="I219">
         <v>30500000</v>
@@ -14058,7 +14030,7 @@
         <v>221</v>
       </c>
       <c r="C220" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D220" t="s">
         <v>112</v>
@@ -14067,13 +14039,13 @@
         <v>2015</v>
       </c>
       <c r="F220" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="G220" t="s">
         <v>94</v>
       </c>
       <c r="H220" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="I220">
         <v>5800000</v>

</xml_diff>